<commit_message>
Revisi IPM Kecamatan Wongsorejo
</commit_message>
<xml_diff>
--- a/Rekap/RekapDimensiKesehatan.xlsx
+++ b/Rekap/RekapDimensiKesehatan.xlsx
@@ -114,11 +114,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0.0"/>
     <numFmt numFmtId="181" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="24">
@@ -157,12 +157,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -171,9 +179,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,74 +242,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,9 +256,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,16 +272,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,13 +309,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,169 +375,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +550,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,6 +562,45 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,54 +623,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -640,139 +643,136 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -791,10 +791,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1417,10 +1417,10 @@
         <v>21</v>
       </c>
       <c r="C19" s="7">
-        <v>69</v>
+        <v>62.5</v>
       </c>
       <c r="D19" s="3">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:4">

</xml_diff>